<commit_message>
finished controlCharts generation for feature Viewport. did testing for failed data, added error handlers. Releasing this version to the insepctors
</commit_message>
<xml_diff>
--- a/examples/Adding Lines Examples.xlsx
+++ b/examples/Adding Lines Examples.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdieckman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\ProcessEngineering\Mark Dieckman\Project Engineer\ML In-Process Tracker\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0B2C8C8-6484-429B-8BF7-4B5A1EB88E3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A317CF6-5F36-4BC4-B04B-9397F70901E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{C9F88BC0-EAE2-43E4-851F-A515F58C1B26}"/>
+    <workbookView xWindow="25080" yWindow="-120" windowWidth="25440" windowHeight="15990" activeTab="1" xr2:uid="{C9F88BC0-EAE2-43E4-851F-A515F58C1B26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Items</t>
   </si>
@@ -65,6 +66,21 @@
   <si>
     <t>Y</t>
   </si>
+  <si>
+    <t>LTOL</t>
+  </si>
+  <si>
+    <t>UTOL</t>
+  </si>
+  <si>
+    <t>UTOL +15%tol</t>
+  </si>
+  <si>
+    <t>UTOL -15%tol</t>
+  </si>
+  <si>
+    <t>LTOL +15%tol</t>
+  </si>
 </sst>
 </file>
 
@@ -82,12 +98,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -102,15 +148,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF66FF99"/>
+      <color rgb="FFFFFF66"/>
+      <color rgb="FFFF5050"/>
+      <color rgb="FF00CC66"/>
+      <color rgb="FFFFCC00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -345,7 +405,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -600,6 +660,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1129843743"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1178,6 +1239,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1242713711"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -1219,6 +1281,1700 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>TOPRED</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E9E8-4BD0-8A48-43EAB9225040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>TOPYELL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF66"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$1:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E9E8-4BD0-8A48-43EAB9225040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>TOPWHITE</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="66FF99">
+                <a:alpha val="86000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$1:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E9E8-4BD0-8A48-43EAB9225040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>BOTTYELL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF66"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$1:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E9E8-4BD0-8A48-43EAB9225040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>BOTTRED</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$1:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E9E8-4BD0-8A48-43EAB9225040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1915705584"/>
+        <c:axId val="1915708496"/>
+      </c:areaChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2606</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2606</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2596</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25940000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2586</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2586</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E9E8-4BD0-8A48-43EAB9225040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1915705584"/>
+        <c:axId val="1915708496"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1915705584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1915708496"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1915708496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.26195000000000002"/>
+          <c:min val="0.25805"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1915705584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>TOPRED</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26195000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4185-43AC-BA97-0E87E7CC6CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>TOPYELL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF66"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$1:$C$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26150000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4185-43AC-BA97-0E87E7CC6CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>TOPGREEN</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="66FF99"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$1:$D$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26105</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4185-43AC-BA97-0E87E7CC6CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>BOTTYELL</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFFF66"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$1:$E$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25895000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4185-43AC-BA97-0E87E7CC6CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>BOTTRED</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF5050"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$1:$F$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.25850000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4185-43AC-BA97-0E87E7CC6CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="13323008"/>
+        <c:axId val="13329248"/>
+      </c:areaChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$A$1:$A$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.26019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2606</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.26040000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26019999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2606</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26079999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26140000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25919999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.25900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.2596</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.25940000000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.2586</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.2586</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25869999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.25879999999999997</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4185-43AC-BA97-0E87E7CC6CA0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="13323008"/>
+        <c:axId val="13329248"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="13323008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="13329248"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="13329248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.26195000000000002"/>
+          <c:min val="0.25805"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="13323008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1343,6 +3099,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
@@ -2321,6 +4157,1038 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2410,6 +5278,83 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{871869DD-4099-4EAF-BE75-E30D9EA52BA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCBAACCE-AE8F-4777-BBB0-ED10192FC34A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>766762</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>604837</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{297C3896-56AF-4833-A306-41E3BF20496A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2730,7 +5675,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -2834,4 +5779,688 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A86DA160-2100-475F-B35F-023E58F84B5C}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A1:M25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.26019999999999999</v>
+      </c>
+      <c r="B1" s="4">
+        <f>$J$4</f>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C1" s="3">
+        <f>$I$2</f>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D1" s="5">
+        <f>$K$4</f>
+        <v>0.26105</v>
+      </c>
+      <c r="E1" s="6">
+        <f>$L$4</f>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F1" s="2">
+        <f>$H$2</f>
+        <v>0.25850000000000001</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0.2606</v>
+      </c>
+      <c r="B2" s="4">
+        <f t="shared" ref="B2:B25" si="0">$J$4</f>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C2" s="3">
+        <f t="shared" ref="C2:C25" si="1">$I$2</f>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D2" s="5">
+        <f t="shared" ref="D2:D25" si="2">$K$4</f>
+        <v>0.26105</v>
+      </c>
+      <c r="E2" s="6">
+        <f t="shared" ref="E2:E25" si="3">$L$4</f>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F2" s="2">
+        <f t="shared" ref="F2:F25" si="4">$H$2</f>
+        <v>0.25850000000000001</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.25850000000000001</v>
+      </c>
+      <c r="I2" s="3">
+        <v>0.26150000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.2606</v>
+      </c>
+      <c r="B3" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E3" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+      <c r="J3" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0.26040000000000002</v>
+      </c>
+      <c r="B4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C4" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E4" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+      <c r="J4" s="4">
+        <f>I2+(I2-H2)*0.15</f>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="K4" s="5">
+        <f>I2-(I2-H2)*0.15</f>
+        <v>0.26105</v>
+      </c>
+      <c r="L4" s="6">
+        <f>H2+(I2-H2)*0.15</f>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="M4">
+        <f>H2-(I2-H2)*0.15</f>
+        <v>0.25805</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0.26019999999999999</v>
+      </c>
+      <c r="B5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C5" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D5" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E5" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0.26</v>
+      </c>
+      <c r="B6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0.26</v>
+      </c>
+      <c r="B7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0.2606</v>
+      </c>
+      <c r="B8" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0.26079999999999998</v>
+      </c>
+      <c r="B9" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.26140000000000002</v>
+      </c>
+      <c r="B10" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C10" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.25919999999999999</v>
+      </c>
+      <c r="B11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C11" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.25919999999999999</v>
+      </c>
+      <c r="B12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C12" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F12" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.25919999999999999</v>
+      </c>
+      <c r="B13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C13" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E13" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F13" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="B14" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C14" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E14" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F14" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.25879999999999997</v>
+      </c>
+      <c r="B15" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C15" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="B16" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C16" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F16" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.2596</v>
+      </c>
+      <c r="B17" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F17" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.25940000000000002</v>
+      </c>
+      <c r="B18" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F18" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.2586</v>
+      </c>
+      <c r="B19" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.2586</v>
+      </c>
+      <c r="B20" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C20" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F20" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="B21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C21" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F21" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.25879999999999997</v>
+      </c>
+      <c r="B22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C22" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F22" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.25879999999999997</v>
+      </c>
+      <c r="B23" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C23" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F23" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0.25879999999999997</v>
+      </c>
+      <c r="B24" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C24" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F24" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0.26</v>
+      </c>
+      <c r="B25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26195000000000002</v>
+      </c>
+      <c r="C25" s="3">
+        <f t="shared" si="1"/>
+        <v>0.26150000000000001</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="2"/>
+        <v>0.26105</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="3"/>
+        <v>0.25895000000000001</v>
+      </c>
+      <c r="F25" s="2">
+        <f t="shared" si="4"/>
+        <v>0.25850000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>